<commit_message>
add new like/ auto publish
</commit_message>
<xml_diff>
--- a/WebBrowser/smzdm.xlsx
+++ b/WebBrowser/smzdm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\smzdm\WebBrowser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiatwang\Documents\GitHub\smzdm\WebBrowser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FB276D-1854-4E99-805B-A398581564B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E499F5-B6AE-4302-892C-FADC658E569D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="155">
   <si>
     <t>phone</t>
   </si>
@@ -431,12 +431,6 @@
     <t>151-160</t>
   </si>
   <si>
-    <t>161-170</t>
-  </si>
-  <si>
-    <t>181-190</t>
-  </si>
-  <si>
     <t>51-60</t>
   </si>
   <si>
@@ -461,49 +455,49 @@
     <t>101-110</t>
   </si>
   <si>
+    <t>111-120</t>
+  </si>
+  <si>
+    <t>122-130</t>
+  </si>
+  <si>
+    <t>131-150</t>
+  </si>
+  <si>
+    <t>91-110</t>
+  </si>
+  <si>
+    <t>101-120</t>
+  </si>
+  <si>
+    <t>121-130</t>
+  </si>
+  <si>
+    <t>50-60</t>
+  </si>
+  <si>
+    <t>40-60</t>
+  </si>
+  <si>
+    <t>71-80</t>
+  </si>
+  <si>
+    <t>150-170</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
-    <t>61-80</t>
+    <t>200-220</t>
+  </si>
+  <si>
+    <t>30-45</t>
+  </si>
+  <si>
+    <t>35-42</t>
   </si>
   <si>
     <t>u</t>
-  </si>
-  <si>
-    <t>81-100</t>
-  </si>
-  <si>
-    <t>111-120</t>
-  </si>
-  <si>
-    <t>122-130</t>
-  </si>
-  <si>
-    <t>131-150</t>
-  </si>
-  <si>
-    <t>111-130</t>
-  </si>
-  <si>
-    <t>190-200</t>
-  </si>
-  <si>
-    <t>171-180</t>
-  </si>
-  <si>
-    <t>91-110</t>
-  </si>
-  <si>
-    <t>101-120</t>
-  </si>
-  <si>
-    <t>221-236</t>
-  </si>
-  <si>
-    <t>237-250</t>
-  </si>
-  <si>
-    <t>121-130</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1569,28 +1563,28 @@
         <v>11</v>
       </c>
       <c r="F2" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="K2" t="s">
         <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="N2" s="1">
         <v>1</v>
@@ -1600,7 +1594,7 @@
       </c>
       <c r="P2" s="1">
         <f>SUM(G2:G35)</f>
-        <v>8400</v>
+        <v>9858</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
@@ -1620,19 +1614,19 @@
         <v>15</v>
       </c>
       <c r="F3" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="K3" t="s">
         <v>80</v>
@@ -1641,7 +1635,7 @@
         <v>78</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
@@ -1664,28 +1658,28 @@
         <v>20</v>
       </c>
       <c r="F4" s="8">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="G4" s="1">
-        <v>158</v>
+        <v>807</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="K4" t="s">
         <v>80</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="N4" s="1">
         <v>1</v>
@@ -1708,10 +1702,10 @@
         <v>22</v>
       </c>
       <c r="F5" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1">
-        <v>110</v>
+        <v>258</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -1729,7 +1723,7 @@
         <v>78</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="N5" s="1">
         <v>1</v>
@@ -1755,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="1">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1770,7 +1764,7 @@
         <v>80</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>127</v>
@@ -1793,10 +1787,10 @@
         <v>25</v>
       </c>
       <c r="F7" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1">
-        <v>1587</v>
+        <v>2509</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -1808,13 +1802,13 @@
         <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="N7" s="1">
         <v>1</v>
@@ -1837,7 +1831,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="1">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -1855,7 +1849,7 @@
         <v>78</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N8" s="1">
         <v>1</v>
@@ -1887,13 +1881,13 @@
         <v>122</v>
       </c>
       <c r="H9" s="1">
-        <v>13</v>
+        <v>-1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
         <v>80</v>
@@ -1902,7 +1896,7 @@
         <v>84</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="N9" s="1">
         <v>1</v>
@@ -1928,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>12</v>
@@ -1943,7 +1937,7 @@
         <v>78</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N10" s="1">
         <v>1</v>
@@ -1963,10 +1957,10 @@
         <v>34</v>
       </c>
       <c r="F11" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -1984,7 +1978,7 @@
         <v>81</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
@@ -2007,13 +2001,13 @@
         <v>21</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="K12" t="s">
         <v>80</v>
@@ -2048,22 +2042,22 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="K13" t="s">
         <v>80</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N13" s="1">
         <v>1</v>
@@ -2089,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>12</v>
@@ -2101,10 +2095,10 @@
         <v>80</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="N14" s="1">
         <v>1</v>
@@ -2133,7 +2127,7 @@
         <v>98</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>12</v>
@@ -2148,7 +2142,7 @@
         <v>78</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="N15" s="1">
         <v>1</v>
@@ -2177,7 +2171,7 @@
         <v>108</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>12</v>
@@ -2192,7 +2186,7 @@
         <v>78</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N16" s="1">
         <v>1</v>
@@ -2224,7 +2218,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>12</v>
@@ -2236,10 +2230,10 @@
         <v>80</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N17" s="1">
         <v>1</v>
@@ -2271,7 +2265,7 @@
         <v>60</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>12</v>
@@ -2286,7 +2280,7 @@
         <v>95</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N18" s="1">
         <v>1</v>
@@ -2318,7 +2312,7 @@
         <v>111</v>
       </c>
       <c r="H19" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>12</v>
@@ -2333,7 +2327,7 @@
         <v>81</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="N19" s="1">
         <v>1</v>
@@ -2365,7 +2359,7 @@
         <v>50</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>12</v>
@@ -2380,7 +2374,7 @@
         <v>78</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="N20" s="1">
         <v>1</v>
@@ -2409,7 +2403,7 @@
         <v>48</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>12</v>
@@ -2424,7 +2418,7 @@
         <v>78</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N21" s="1">
         <v>1</v>
@@ -2444,25 +2438,25 @@
         <v>13</v>
       </c>
       <c r="G22" s="1">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="H22" s="1">
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="K22" t="s">
         <v>80</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="N22" s="1">
         <v>1</v>
@@ -2485,13 +2479,13 @@
         <v>183</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="K23" t="s">
         <v>80</v>
@@ -2500,7 +2494,7 @@
         <v>84</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N23" s="1">
         <v>1</v>
@@ -2529,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>12</v>
@@ -2544,7 +2538,7 @@
         <v>129</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N24" s="1">
         <v>1</v>
@@ -2570,13 +2564,13 @@
         <v>4979</v>
       </c>
       <c r="H25" s="1">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>140</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s">
         <v>80</v>
@@ -2585,7 +2579,7 @@
         <v>81</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="N25" s="1">
         <v>1</v>
@@ -2614,7 +2608,7 @@
         <v>44</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>12</v>
@@ -2626,10 +2620,10 @@
         <v>80</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="N26" s="1">
         <v>1</v>
@@ -2656,7 +2650,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>12</v>
@@ -2671,7 +2665,7 @@
         <v>78</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="N27" s="1">
         <v>1</v>
@@ -2700,13 +2694,13 @@
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>16</v>
+        <v>-1</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="K28" t="s">
         <v>80</v>
@@ -2715,7 +2709,7 @@
         <v>84</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N28" s="1">
         <v>1</v>
@@ -2738,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>68</v>
@@ -2782,13 +2776,13 @@
         <v>44</v>
       </c>
       <c r="H30" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>68</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="K30" t="s">
         <v>80</v>
@@ -2820,13 +2814,13 @@
         <v>20</v>
       </c>
       <c r="H31" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>68</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="K31" t="s">
         <v>80</v>
@@ -2858,7 +2852,7 @@
         <v>18</v>
       </c>
       <c r="H32" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>68</v>
@@ -2870,10 +2864,10 @@
         <v>80</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="N32" s="1">
         <v>1</v>
@@ -2893,25 +2887,25 @@
         <v>6</v>
       </c>
       <c r="G33" s="1">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="H33" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="K33" t="s">
         <v>80</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="N33" s="1">
         <v>1</v>
@@ -2934,7 +2928,7 @@
         <v>18</v>
       </c>
       <c r="H34" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>68</v>

</xml_diff>